<commit_message>
More of the application skeleton added, including CLI and packaging. Currently works for tiling the basic "Standalone Template" project using wall-to-wall config file.
</commit_message>
<xml_diff>
--- a/docs/config_parsing_and_defaults.xlsx
+++ b/docs/config_parsing_and_defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\projects\gcbmwalltowall\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F92800-F733-4C2A-B09B-E3527BC28313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47C7B29-55D1-4FCF-8022-2FFE6D610BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1605" windowWidth="28800" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +723,7 @@
     <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="67" style="2" customWidth="1"/>
+    <col min="6" max="6" width="50.85546875" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1321,10 +1321,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Now tiles disturbances, with detection of year and disturbance type attributes if not specified.
</commit_message>
<xml_diff>
--- a/docs/config_parsing_and_defaults.xlsx
+++ b/docs/config_parsing_and_defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\projects\gcbmwalltowall\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47C7B29-55D1-4FCF-8022-2FFE6D610BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3DBD9D-41FD-467E-9B50-0C9EB6DA82B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1605" windowWidth="28800" windowHeight="15315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="7005" windowWidth="28800" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented spatial rollback, with some supporting changes in other components.
</commit_message>
<xml_diff>
--- a/docs/config_parsing_and_defaults.xlsx
+++ b/docs/config_parsing_and_defaults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\projects\gcbmwalltowall\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3DBD9D-41FD-467E-9B50-0C9EB6DA82B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1134AFDD-B97C-4AE9-9571-EDD9A66C8331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7005" windowWidth="28800" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="465" yWindow="1140" windowWidth="22995" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="114">
   <si>
     <t>Section</t>
   </si>
@@ -364,6 +364,9 @@
   </si>
   <si>
     <t>Use 1990 as default value.</t>
+  </si>
+  <si>
+    <t>Use as full layer definition for the inventory vintage layer.</t>
   </si>
 </sst>
 </file>
@@ -710,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,10 +1797,13 @@
         <v>46</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1805,19 +1811,16 @@
         <v>101</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1831,9 +1834,29 @@
         <v>47</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="E60" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Disturbance layers now accept a path to a specific lookup table.
Can now use the special keyword "filename" for the "year" part of a disturbance layer in order to force parsing the year from the filename.
</commit_message>
<xml_diff>
--- a/docs/config_parsing_and_defaults.xlsx
+++ b/docs/config_parsing_and_defaults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\projects\gcbmwalltowall\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03826951-443E-4420-ABE6-66A6ECFA72C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D471F5-409B-4BE1-814C-D3E0CADBB1AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15165" yWindow="2160" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="127">
   <si>
     <t>Section</t>
   </si>
@@ -252,9 +252,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>Use as name of attribute containing year of disturbance.</t>
-  </si>
-  <si>
     <t>Ensure attribute exists in layer.</t>
   </si>
   <si>
@@ -403,6 +400,12 @@
   </si>
   <si>
     <t>Use as path to age distribution JSON or Excel file for rollback tool.</t>
+  </si>
+  <si>
+    <t>Use as name of attribute containing year of disturbance, or if special "filename" keyword is used, try to parse year from filename.</t>
+  </si>
+  <si>
+    <t>Ensure attribute exists in layer or year is parseable from filename.</t>
   </si>
 </sst>
 </file>
@@ -751,8 +754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +914,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -928,10 +931,10 @@
         <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1298,7 +1301,7 @@
         <v>10</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1355,7 +1358,7 @@
         <v>10</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1469,7 +1472,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
@@ -1483,10 +1486,10 @@
         <v>5</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1503,10 +1506,10 @@
         <v>36</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1523,7 +1526,7 @@
         <v>10</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1531,7 +1534,7 @@
         <v>73</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>46</v>
@@ -1540,10 +1543,10 @@
         <v>5</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1551,7 +1554,7 @@
         <v>73</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>46</v>
@@ -1560,10 +1563,10 @@
         <v>5</v>
       </c>
       <c r="E43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1571,7 +1574,7 @@
         <v>73</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>46</v>
@@ -1580,7 +1583,7 @@
         <v>10</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1588,7 +1591,7 @@
         <v>73</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>46</v>
@@ -1597,10 +1600,10 @@
         <v>5</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1608,7 +1611,7 @@
         <v>73</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>46</v>
@@ -1617,10 +1620,10 @@
         <v>36</v>
       </c>
       <c r="E46" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1628,7 +1631,7 @@
         <v>73</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>46</v>
@@ -1637,7 +1640,7 @@
         <v>10</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1645,7 +1648,7 @@
         <v>73</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>46</v>
@@ -1654,10 +1657,10 @@
         <v>5</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1665,7 +1668,7 @@
         <v>73</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>46</v>
@@ -1674,10 +1677,10 @@
         <v>36</v>
       </c>
       <c r="E49" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -1685,7 +1688,7 @@
         <v>73</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>46</v>
@@ -1694,7 +1697,7 @@
         <v>10</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1702,7 +1705,7 @@
         <v>6</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>46</v>
@@ -1711,7 +1714,7 @@
         <v>40</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1719,7 +1722,7 @@
         <v>6</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>46</v>
@@ -1728,15 +1731,15 @@
         <v>10</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>45</v>
@@ -1745,7 +1748,7 @@
         <v>5</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>24</v>
@@ -1753,10 +1756,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>45</v>
@@ -1765,15 +1768,15 @@
         <v>10</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>45</v>
@@ -1782,18 +1785,18 @@
         <v>36</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>45</v>
@@ -1802,7 +1805,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>24</v>
@@ -1810,10 +1813,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>45</v>
@@ -1822,7 +1825,7 @@
         <v>49</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>51</v>
@@ -1830,10 +1833,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>45</v>
@@ -1842,15 +1845,15 @@
         <v>10</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>46</v>
@@ -1859,18 +1862,18 @@
         <v>36</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>46</v>
@@ -1879,32 +1882,32 @@
         <v>10</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="E61" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>46</v>
@@ -1913,32 +1916,32 @@
         <v>10</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>46</v>
@@ -1947,15 +1950,15 @@
         <v>10</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>46</v>
@@ -1964,18 +1967,18 @@
         <v>5</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>46</v>
@@ -1984,15 +1987,15 @@
         <v>10</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>46</v>
@@ -2001,18 +2004,18 @@
         <v>5</v>
       </c>
       <c r="E67" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>46</v>
@@ -2021,7 +2024,7 @@
         <v>10</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>